<commit_message>
keywords bearbeitet und an G.Sliwniski abgeschickt
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maciejwlasniak/Documents/Oberseminar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D049691-79C4-1249-9B31-73FD09FD53A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C339AF-9FA8-964D-8983-2020E3D8103F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28060" yWindow="12100" windowWidth="28040" windowHeight="17360" xr2:uid="{5D602128-0DC1-984E-AEC0-D4C4A75FD006}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="17920" windowHeight="21440" xr2:uid="{5D602128-0DC1-984E-AEC0-D4C4A75FD006}"/>
   </bookViews>
   <sheets>
     <sheet name="Keywods" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>robot</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Thema:</t>
   </si>
   <si>
-    <t>Voraussetzung für Einbinden von REHA-Roboten in der klinischen Praxis aus Sicht von Physioterapeuten.</t>
-  </si>
-  <si>
     <t>application</t>
   </si>
   <si>
@@ -116,13 +113,25 @@
   </si>
   <si>
     <t>kinematics</t>
+  </si>
+  <si>
+    <t>therapy</t>
+  </si>
+  <si>
+    <t>clinical</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>Requirements for the successful integration of rehabilitation robots in (physiotherapeutical) clinic routines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,8 +140,39 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +182,22 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,15 +211,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Dobry" xfId="1" builtinId="26"/>
+    <cellStyle name="Hiperłącze" xfId="3" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Zły" xfId="2" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -475,37 +542,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F94A405-DDCA-1048-AE0C-7B0A416A1B6E}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="12.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -514,75 +584,86 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -601,11 +682,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>18</v>
+      <c r="A2" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://ieeexplore.ieee.org/search/searchresult.jsp?action=search&amp;newsearch=true&amp;matchBoolean=true&amp;queryText=((((((%22All%20Metadata%22:robot)%20AND%20%22All%20Metadata%22:rehabilitation)%20NOT%20%22All%20Metadata%22:control)%20AND%20%22All%20Metadata%22:application)%20NOT%20%22All%20Metadata%22:algorithm)%20NOT%20%22All%20Metadata%22:humanoid)&amp;ranges=1872_2021_Year&amp;highlight=true&amp;returnFacets=ALL&amp;returnType=SEARCH&amp;matchPubs=true&amp;pageNumber=11" xr:uid="{ED7DCC42-09C5-6548-8F78-A50191CAD828}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>